<commit_message>
Updated ASV bubbleplot class v1 annotated.pptx and ASV bubbleplot class v1 annotated.png with correct post hocs. Updated sig.asvs.v2.csv with correct otu order. Updated sig.asvs.blast.data.xlsx with blast data and relevant papers.
</commit_message>
<xml_diff>
--- a/output/sig.asvs.blast.data.xlsx
+++ b/output/sig.asvs.blast.data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesle\Documents\University of Hawaii\Nelson Lab\Experiments+Field Ops\ABCDom\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{095867BE-81AD-46FE-AC79-8F89D959D826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8738A22A-EE18-45BE-8AEC-1500D65E1F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3FB00573-87FA-4C84-9822-A3D5F19B315B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="207">
   <si>
     <t>Otu00368</t>
   </si>
@@ -602,16 +602,78 @@
   </si>
   <si>
     <t>uncultured Pseudoalteromonas</t>
+  </si>
+  <si>
+    <t>https://www.microbiologyresearch.org/content/journal/ijsem/10.1099/ijsem.0.003533</t>
+  </si>
+  <si>
+    <t>https://journals.asm.org/doi/10.1128/AEM.02852-15</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>copiotroph</t>
+  </si>
+  <si>
+    <t>this strain found in oligotrophic waters</t>
+  </si>
+  <si>
+    <t>blast_hit</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/nucleotide/MK224685.1?report=genbank&amp;log$=nucltop&amp;blast_rank=35&amp;RID=6SKME8AW01N</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s00338-021-02062-5\, https://www.frontiersin.org/articles/10.3389/fmicb.2019.01850/full, https://link.springer.com/article/10.1007/s00248-010-9644-3</t>
+  </si>
+  <si>
+    <t>induce coral larval settlement, diseased coral n cca</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/nucleotide/KY278213.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=6SWX65D6013</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary-wiley-com.eres.library.manoa.hawaii.edu/doi/full/10.1111/maec.12474</t>
+  </si>
+  <si>
+    <t>Flavobacterium associated with particle associated algal bloom</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/nucleotide/KU560494.1?report=genbank&amp;log$=nucltop&amp;blast_rank=2&amp;RID=6SXVVRS8013</t>
+  </si>
+  <si>
+    <t>https://www.frontiersin.org/articles/10.3389/fmicb.2016.00316/full, https://www.nature.com/articles/nrmicro1635, https://www.microbiologyresearch.org/content/journal/ijsem/10.1099/ijs.0.63800-0</t>
+  </si>
+  <si>
+    <t>isolated from macroalgae, can induce coral white syndrome like symptoms. This genus has been documented to cause white disease in other corals</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/nucleotide/MN335274.1?report=genbank&amp;log$=nucltop&amp;blast_rank=2&amp;RID=6T65K102013</t>
+  </si>
+  <si>
+    <t>https://journals.plos.org/plosone/article?id=10.1371/journal.pone.0188319</t>
+  </si>
+  <si>
+    <t>mcap pathogen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -634,14 +696,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -954,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA214FDF-695F-4524-B2F1-1E4ECCC4809A}">
-  <dimension ref="A1:Y32"/>
+  <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X33" sqref="X33"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -966,9 +1031,11 @@
     <col min="22" max="22" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="36.90625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.26953125" customWidth="1"/>
+    <col min="26" max="26" width="23.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -1044,37 +1111,43 @@
       <c r="Y1" t="s">
         <v>136</v>
       </c>
+      <c r="Z1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>191</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2">
-        <v>2.5946584657060399E-4</v>
-      </c>
-      <c r="C2">
-        <v>4.3367862926800898E-3</v>
+        <v>108</v>
+      </c>
+      <c r="B2" s="1">
+        <v>7.2645747956430099E-25</v>
+      </c>
+      <c r="C2" s="1">
+        <v>8.4995525109023298E-23</v>
       </c>
       <c r="D2" s="1">
-        <v>3.2949222009669098E-5</v>
-      </c>
-      <c r="E2">
-        <v>7.15468820781387E-4</v>
-      </c>
-      <c r="F2">
-        <v>1.42342775562572E-2</v>
-      </c>
-      <c r="G2">
-        <v>0.120200566030617</v>
+        <v>2.0480265280941298E-24</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3.1130003227030799E-22</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1.8435208765420901E-22</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2.8021517323439703E-20</v>
       </c>
       <c r="H2">
-        <v>1.29277094401242</v>
+        <v>25.799031949536499</v>
       </c>
       <c r="I2">
-        <v>1.4689689194295801</v>
+        <v>25.541920612953898</v>
       </c>
       <c r="J2">
-        <v>0.775714091420313</v>
+        <v>22.460961767105299</v>
       </c>
       <c r="K2" t="s">
         <v>2</v>
@@ -1083,13 +1156,13 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N2" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="O2" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="P2" t="s">
         <v>4</v>
@@ -1107,48 +1180,51 @@
         <v>8</v>
       </c>
       <c r="U2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="V2" t="s">
-        <v>137</v>
+        <v>177</v>
       </c>
       <c r="W2" t="s">
-        <v>139</v>
-      </c>
-      <c r="X2" s="1">
-        <v>3E-52</v>
+        <v>178</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3">
-        <v>1.1059093160460101E-3</v>
-      </c>
-      <c r="C3">
-        <v>1.2939138997738299E-2</v>
-      </c>
-      <c r="D3">
-        <v>4.60154160653772E-3</v>
-      </c>
-      <c r="E3">
-        <v>3.5693556476693498E-2</v>
-      </c>
-      <c r="F3">
-        <v>2.0240163024394301E-2</v>
-      </c>
-      <c r="G3">
-        <v>0.15382523898539599</v>
+        <v>82</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4.0166138013074299E-8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.5664793825099E-6</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.5798540859477E-9</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6.00344552660125E-8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>7.1257924430440104E-7</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2.7078011283567201E-5</v>
       </c>
       <c r="H3">
-        <v>-1.15038439018938</v>
+        <v>9.8472328222506906</v>
       </c>
       <c r="I3">
-        <v>-0.99083638959763498</v>
+        <v>10.7926616939578</v>
       </c>
       <c r="J3">
-        <v>-0.72391589169332404</v>
+        <v>8.3623201898607995</v>
       </c>
       <c r="K3" t="s">
         <v>2</v>
@@ -1157,13 +1233,13 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="O3" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="P3" t="s">
         <v>4</v>
@@ -1175,69 +1251,78 @@
         <v>6</v>
       </c>
       <c r="S3" t="s">
-        <v>105</v>
+        <v>7</v>
       </c>
       <c r="T3" t="s">
-        <v>106</v>
+        <v>59</v>
       </c>
       <c r="U3" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="V3" t="s">
-        <v>140</v>
+        <v>186</v>
       </c>
       <c r="W3" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="X3" s="1">
-        <v>2.0000000000000001E-127</v>
+        <v>7.9999999999999996E-126</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4">
-        <v>7.7721414886593093E-2</v>
+        <v>84</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4.3944727825824598E-5</v>
       </c>
       <c r="C4">
-        <v>0.39403838801529101</v>
-      </c>
-      <c r="D4">
-        <v>6.6966251935410303E-4</v>
+        <v>8.5692219260358096E-4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2.0440309336398101E-5</v>
       </c>
       <c r="E4">
-        <v>7.2706216387016902E-3</v>
+        <v>5.6101139809715695E-4</v>
       </c>
       <c r="F4">
-        <v>0.802801862068799</v>
+        <v>2.7061485275990899E-4</v>
       </c>
       <c r="G4">
-        <v>0.99734399315384603</v>
+        <v>5.1416822024382804E-3</v>
       </c>
       <c r="H4">
-        <v>-1.2939683480611199</v>
+        <v>10.0440404270764</v>
       </c>
       <c r="I4">
-        <v>-2.4960304829707498</v>
+        <v>10.459349191909601</v>
       </c>
       <c r="J4">
-        <v>0.16291296848838199</v>
+        <v>8.2325208374458594</v>
       </c>
       <c r="K4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4" t="s">
         <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N4" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="O4" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="P4" t="s">
         <v>4</v>
@@ -1249,140 +1334,140 @@
         <v>6</v>
       </c>
       <c r="S4" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="T4" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="U4" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="V4" t="s">
-        <v>141</v>
+        <v>187</v>
       </c>
       <c r="W4" t="s">
-        <v>142</v>
+        <v>188</v>
       </c>
       <c r="X4" s="1">
         <v>2.0000000000000001E-127</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5">
-        <v>0.15046919958421101</v>
-      </c>
-      <c r="C5">
-        <v>0.50299703861007805</v>
+        <v>94</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.0977287867893E-9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6.4217134027174294E-8</v>
       </c>
       <c r="D5" s="1">
-        <v>9.2015719344879594E-5</v>
-      </c>
-      <c r="E5">
-        <v>1.7482986675527101E-3</v>
-      </c>
-      <c r="F5">
-        <v>4.2026271586780697E-2</v>
-      </c>
-      <c r="G5">
-        <v>0.24569204927656399</v>
+        <v>4.5243470905563701E-11</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2.2923358592152299E-9</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4.3596222344221402E-11</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2.20887526544055E-9</v>
       </c>
       <c r="H5">
-        <v>-0.71432114294556903</v>
+        <v>22.8658566406198</v>
       </c>
       <c r="I5">
-        <v>-1.94391886793681</v>
+        <v>24.670600574976199</v>
       </c>
       <c r="J5">
-        <v>-0.89870437805570702</v>
+        <v>22.364748216294</v>
       </c>
       <c r="K5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L5" t="s">
         <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N5" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="O5" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="P5" t="s">
         <v>4</v>
       </c>
       <c r="Q5" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="R5" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="S5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="T5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="U5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="V5" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="W5" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1.81670746614665E-5</v>
+        <v>90</v>
+      </c>
+      <c r="B6">
+        <v>2.5946584657060399E-4</v>
       </c>
       <c r="C6">
-        <v>4.2510954707831701E-4</v>
-      </c>
-      <c r="D6">
-        <v>0.104153359670923</v>
+        <v>4.3367862926800898E-3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.2949222009669098E-5</v>
       </c>
       <c r="E6">
-        <v>0.38612952853610399</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1.0148616726825199E-5</v>
+        <v>7.15468820781387E-4</v>
+      </c>
+      <c r="F6">
+        <v>1.42342775562572E-2</v>
       </c>
       <c r="G6">
-        <v>2.5709829041290502E-4</v>
+        <v>0.120200566030617</v>
       </c>
       <c r="H6">
-        <v>1.56096437704983</v>
+        <v>1.29277094401242</v>
       </c>
       <c r="I6">
-        <v>0.59153829644759404</v>
+        <v>1.4689689194295801</v>
       </c>
       <c r="J6">
-        <v>1.43412807510652</v>
+        <v>0.775714091420313</v>
       </c>
       <c r="K6" t="s">
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="O6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="P6" t="s">
         <v>4</v>
@@ -1400,122 +1485,131 @@
         <v>8</v>
       </c>
       <c r="U6" t="s">
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="V6" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="W6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="X6" s="1">
-        <v>2.0000000000000001E-127</v>
+        <v>3E-52</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B7">
-        <v>5.0136967292487003E-3</v>
+        <v>1.1059093160460101E-3</v>
       </c>
       <c r="C7">
-        <v>4.8883543110174899E-2</v>
+        <v>1.2939138997738299E-2</v>
       </c>
       <c r="D7">
-        <v>0.58684774093238001</v>
+        <v>4.60154160653772E-3</v>
       </c>
       <c r="E7">
-        <v>0.93116326736450294</v>
+        <v>3.5693556476693498E-2</v>
       </c>
       <c r="F7">
-        <v>5.56907506857603E-2</v>
+        <v>2.0240163024394301E-2</v>
       </c>
       <c r="G7">
-        <v>0.30251259505272599</v>
+        <v>0.15382523898539599</v>
       </c>
       <c r="H7">
-        <v>-2.5236120599264602</v>
+        <v>-1.15038439018938</v>
       </c>
       <c r="I7">
-        <v>-0.48206625802529601</v>
+        <v>-0.99083638959763498</v>
       </c>
       <c r="J7">
-        <v>-1.51871658779463</v>
+        <v>-0.72391589169332404</v>
       </c>
       <c r="K7" t="s">
         <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M7" t="s">
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="O7" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P7" t="s">
         <v>4</v>
       </c>
       <c r="Q7" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="R7" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="S7" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="T7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="U7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="V7" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="W7" t="s">
-        <v>148</v>
+        <v>143</v>
+      </c>
+      <c r="X7" s="1">
+        <v>2.0000000000000001E-127</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="B8">
-        <v>1.59419095125224E-2</v>
+        <v>1.2585940312723001E-3</v>
       </c>
       <c r="C8">
-        <v>0.11657521331032</v>
+        <v>1.3386863787169001E-2</v>
       </c>
       <c r="D8">
-        <v>4.7339319761837301E-4</v>
+        <v>1.14850042808921E-4</v>
       </c>
       <c r="E8">
-        <v>5.5350589259994401E-3</v>
+        <v>1.93968961188399E-3</v>
       </c>
       <c r="F8">
-        <v>7.1683472380685903E-3</v>
+        <v>2.4773417768380501E-2</v>
       </c>
       <c r="G8">
-        <v>6.8099298761651605E-2</v>
+        <v>0.16371997829538501</v>
       </c>
       <c r="H8">
-        <v>2.5525300669321198</v>
+        <v>1.36904978364584</v>
       </c>
       <c r="I8">
-        <v>3.6992945352937099</v>
+        <v>1.62233707278777</v>
       </c>
       <c r="J8">
-        <v>2.5459242730252698</v>
+        <v>0.84556336159601597</v>
       </c>
       <c r="K8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" t="s">
         <v>2</v>
@@ -1524,10 +1618,10 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="O8" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="P8" t="s">
         <v>4</v>
@@ -1542,66 +1636,69 @@
         <v>7</v>
       </c>
       <c r="T8" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="U8" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="V8" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="W8" t="s">
-        <v>150</v>
-      </c>
-      <c r="X8" s="1">
-        <v>2.0000000000000001E-127</v>
+        <v>157</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9">
-        <v>2.7351902338559501E-2</v>
+        <v>96</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.81670746614665E-5</v>
       </c>
       <c r="C9">
-        <v>0.16843013545323501</v>
+        <v>4.2510954707831701E-4</v>
       </c>
       <c r="D9">
-        <v>3.1860298969465302E-4</v>
+        <v>0.104153359670923</v>
       </c>
       <c r="E9">
-        <v>4.0356378694656001E-3</v>
-      </c>
-      <c r="F9">
-        <v>2.3968772804732901E-2</v>
+        <v>0.38612952853610399</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.0148616726825199E-5</v>
       </c>
       <c r="G9">
-        <v>0.16371997829538501</v>
+        <v>2.5709829041290502E-4</v>
       </c>
       <c r="H9">
-        <v>1.96513005696655</v>
+        <v>1.56096437704983</v>
       </c>
       <c r="I9">
-        <v>3.2030747455898201</v>
+        <v>0.59153829644759404</v>
       </c>
       <c r="J9">
-        <v>1.79727972128311</v>
+        <v>1.43412807510652</v>
       </c>
       <c r="K9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N9" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="O9" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="P9" t="s">
         <v>4</v>
@@ -1616,122 +1713,128 @@
         <v>7</v>
       </c>
       <c r="T9" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="U9" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="V9" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="W9" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="X9" s="1">
         <v>2.0000000000000001E-127</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10">
-        <v>1.2817162989086099E-2</v>
-      </c>
-      <c r="C10">
-        <v>9.9973871314871704E-2</v>
+        <v>86</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.03470931453534E-7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3.0265247450158599E-6</v>
       </c>
       <c r="D10">
-        <v>1.65429974700948E-4</v>
+        <v>0.25330807448201498</v>
       </c>
       <c r="E10">
-        <v>2.2859414685949199E-3</v>
-      </c>
-      <c r="F10">
-        <v>3.7030354202105001E-2</v>
-      </c>
-      <c r="G10">
-        <v>0.23452557661333201</v>
+        <v>0.71755221760155696</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4.77327487954768E-13</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3.62768890845624E-11</v>
       </c>
       <c r="H10">
-        <v>2.18507826299735</v>
+        <v>-8.9778405311703597</v>
       </c>
       <c r="I10">
-        <v>3.2942001927592499</v>
+        <v>1.0022527076032399</v>
       </c>
       <c r="J10">
-        <v>1.6339460315015999</v>
+        <v>-10.2292363423296</v>
       </c>
       <c r="K10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="O10" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="P10" t="s">
         <v>4</v>
       </c>
       <c r="Q10" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="R10" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="S10" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="T10" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="U10" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="V10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="W10" t="s">
         <v>145</v>
       </c>
+      <c r="Y10" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>192</v>
+      </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1.03470931453534E-7</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3.0265247450158599E-6</v>
+        <v>110</v>
+      </c>
+      <c r="B11">
+        <v>5.2296258790457699E-4</v>
+      </c>
+      <c r="C11">
+        <v>6.7985136427595001E-3</v>
       </c>
       <c r="D11">
-        <v>0.25330807448201498</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0.71755221760155696</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1">
-        <v>4.77327487954768E-13</v>
-      </c>
-      <c r="G11" s="1">
-        <v>3.62768890845624E-11</v>
+        <v>3.5239219193501199E-5</v>
+      </c>
+      <c r="G11">
+        <v>7.6519447391602705E-4</v>
       </c>
       <c r="H11">
-        <v>-8.9778405311703597</v>
+        <v>9.5195379091599097</v>
       </c>
       <c r="I11">
-        <v>1.0022527076032399</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>-10.2292363423296</v>
+        <v>10.366478918685701</v>
       </c>
       <c r="K11" t="s">
         <v>2</v>
@@ -1743,10 +1846,10 @@
         <v>2</v>
       </c>
       <c r="N11" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="O11" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="P11" t="s">
         <v>4</v>
@@ -1761,418 +1864,445 @@
         <v>7</v>
       </c>
       <c r="T11" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="U11" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="V11" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="W11" t="s">
-        <v>145</v>
+        <v>150</v>
+      </c>
+      <c r="X11" s="1">
+        <v>7.9999999999999996E-126</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="B12">
-        <v>0.32671958514110599</v>
+        <v>3.46876620281595E-4</v>
       </c>
       <c r="C12">
-        <v>0.69627656975421404</v>
+        <v>5.0730705716183298E-3</v>
       </c>
       <c r="D12">
-        <v>4.9313466184905501E-3</v>
+        <v>1.9624727020539499E-2</v>
       </c>
       <c r="E12">
-        <v>3.5693556476693498E-2</v>
+        <v>0.110479944708223</v>
       </c>
       <c r="F12">
-        <v>0.19886179858355699</v>
+        <v>6.05096876389656E-4</v>
       </c>
       <c r="G12">
-        <v>0.82528948433412697</v>
+        <v>1.02194139123586E-2</v>
       </c>
       <c r="H12">
-        <v>0.77767918783579904</v>
+        <v>1.8204520432071301</v>
       </c>
       <c r="I12">
-        <v>2.2213888527322601</v>
+        <v>1.1835626076852099</v>
       </c>
       <c r="J12">
-        <v>0.908460508709656</v>
+        <v>1.5508191015553201</v>
       </c>
       <c r="K12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="O12" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="P12" t="s">
         <v>4</v>
       </c>
       <c r="Q12" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="R12" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="S12" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="T12" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="U12" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="V12" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="W12" t="s">
         <v>145</v>
       </c>
+      <c r="Y12" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>200</v>
+      </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B13">
-        <v>1.2585940312723001E-3</v>
+        <v>5.0136967292487003E-3</v>
       </c>
       <c r="C13">
-        <v>1.3386863787169001E-2</v>
+        <v>4.8883543110174899E-2</v>
       </c>
       <c r="D13">
-        <v>1.14850042808921E-4</v>
+        <v>0.58684774093238001</v>
       </c>
       <c r="E13">
-        <v>1.93968961188399E-3</v>
+        <v>0.93116326736450294</v>
       </c>
       <c r="F13">
-        <v>2.4773417768380501E-2</v>
+        <v>5.56907506857603E-2</v>
       </c>
       <c r="G13">
-        <v>0.16371997829538501</v>
+        <v>0.30251259505272599</v>
       </c>
       <c r="H13">
-        <v>1.36904978364584</v>
+        <v>-2.5236120599264602</v>
       </c>
       <c r="I13">
-        <v>1.62233707278777</v>
+        <v>-0.48206625802529601</v>
       </c>
       <c r="J13">
-        <v>0.84556336159601597</v>
+        <v>-1.51871658779463</v>
       </c>
       <c r="K13" t="s">
         <v>2</v>
       </c>
       <c r="L13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M13" t="s">
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="P13" t="s">
         <v>4</v>
       </c>
       <c r="Q13" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="R13" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="S13" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="T13" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="U13" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
       <c r="V13" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="W13" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B14">
-        <v>3.46876620281595E-4</v>
-      </c>
-      <c r="C14">
-        <v>5.0730705716183298E-3</v>
+        <v>8.5320776887851096E-3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>1.9624727020539499E-2</v>
+        <v>3.48720690711513E-3</v>
       </c>
       <c r="E14">
-        <v>0.110479944708223</v>
+        <v>3.11797323459705E-2</v>
       </c>
       <c r="F14">
-        <v>6.05096876389656E-4</v>
+        <v>1.71192850067222E-3</v>
       </c>
       <c r="G14">
-        <v>1.02194139123586E-2</v>
+        <v>2.36557392820161E-2</v>
       </c>
       <c r="H14">
-        <v>1.8204520432071301</v>
+        <v>8.2400067398754295</v>
       </c>
       <c r="I14">
-        <v>1.1835626076852099</v>
+        <v>9.1230836510590603</v>
       </c>
       <c r="J14">
-        <v>1.5508191015553201</v>
+        <v>8.9116972443720694</v>
       </c>
       <c r="K14" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14" t="s">
         <v>2</v>
       </c>
       <c r="N14" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="O14" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="P14" t="s">
         <v>4</v>
       </c>
       <c r="Q14" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="R14" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="S14" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="T14" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="U14" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="V14" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="W14" t="s">
-        <v>145</v>
+        <v>181</v>
+      </c>
+      <c r="X14" s="1">
+        <v>2.0000000000000001E-127</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1.0977287867893E-9</v>
-      </c>
-      <c r="C15" s="1">
-        <v>6.4217134027174294E-8</v>
-      </c>
-      <c r="D15" s="1">
-        <v>4.5243470905563701E-11</v>
-      </c>
-      <c r="E15" s="1">
-        <v>2.2923358592152299E-9</v>
-      </c>
-      <c r="F15" s="1">
-        <v>4.3596222344221402E-11</v>
-      </c>
-      <c r="G15" s="1">
-        <v>2.20887526544055E-9</v>
+        <v>78</v>
+      </c>
+      <c r="B15">
+        <v>0.63830387749305495</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>4.8476849803422897E-3</v>
+      </c>
+      <c r="E15">
+        <v>3.5693556476693498E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.67130103556288401</v>
+      </c>
+      <c r="G15">
+        <v>0.99734399315384603</v>
       </c>
       <c r="H15">
-        <v>22.8658566406198</v>
+        <v>-1.1582210283757299</v>
       </c>
       <c r="I15">
-        <v>24.670600574976199</v>
+        <v>-7.98886589803897</v>
       </c>
       <c r="J15">
-        <v>22.364748216294</v>
+        <v>-0.92871427344596602</v>
       </c>
       <c r="K15" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L15" t="s">
         <v>2</v>
       </c>
       <c r="M15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="O15" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="P15" t="s">
         <v>4</v>
       </c>
       <c r="Q15" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="R15" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="S15" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="T15" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="U15" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="V15" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="W15" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="B16">
-        <v>2.3926605713549001E-2</v>
+        <v>0.73087028011701705</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
       <c r="D16">
-        <v>1.0912925960678801E-2</v>
+        <v>1.54082605663626E-3</v>
       </c>
       <c r="E16">
-        <v>7.5398397546507803E-2</v>
+        <v>1.5381297540471101E-2</v>
       </c>
       <c r="F16">
-        <v>3.7964934956685099E-3</v>
+        <v>0.72874036337219805</v>
       </c>
       <c r="G16">
-        <v>3.8471134089440903E-2</v>
+        <v>0.99734399315384603</v>
       </c>
       <c r="H16">
-        <v>7.3093565963403604</v>
+        <v>-0.58724321488165099</v>
       </c>
       <c r="I16">
-        <v>8.1937535691923404</v>
+        <v>-6.9757384231914203</v>
       </c>
       <c r="J16">
-        <v>8.4641318944150807</v>
+        <v>0.51828966748271599</v>
       </c>
       <c r="K16" t="s">
         <v>10</v>
       </c>
       <c r="L16" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="O16" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="P16" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="Q16" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="R16" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="S16" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="T16" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="U16" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="V16" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="W16" t="s">
-        <v>161</v>
+        <v>184</v>
+      </c>
+      <c r="X16" t="s">
+        <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="B17">
-        <v>0.18115724139428399</v>
-      </c>
-      <c r="C17">
-        <v>0.52988493107828105</v>
+        <v>0.68913736661825598</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
       </c>
       <c r="D17">
-        <v>5.0265572576471899E-2</v>
+        <v>1.61908395162854E-3</v>
       </c>
       <c r="E17">
-        <v>0.231526273685568</v>
+        <v>1.5381297540471101E-2</v>
       </c>
       <c r="F17">
-        <v>2.5200208004161201E-3</v>
+        <v>0.87396767139879195</v>
       </c>
       <c r="G17">
-        <v>2.9464858589480801E-2</v>
+        <v>0.99734399315384603</v>
       </c>
       <c r="H17">
-        <v>0.92791339438389997</v>
+        <v>-0.68745418612221099</v>
       </c>
       <c r="I17">
-        <v>-1.3818296697146699</v>
+        <v>-6.9635184693634002</v>
       </c>
       <c r="J17">
-        <v>1.8550138623057999</v>
+        <v>0.23838138054142299</v>
       </c>
       <c r="K17" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="O17" t="s">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="P17" t="s">
         <v>4</v>
@@ -2193,131 +2323,128 @@
         <v>9</v>
       </c>
       <c r="V17" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="W17" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B18">
-        <v>0.16668498818429101</v>
-      </c>
-      <c r="C18">
-        <v>0.520079900515794</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2.2145186766993099E-5</v>
+        <v>2.3926605713549001E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>1.0912925960678801E-2</v>
       </c>
       <c r="E18">
-        <v>5.6101139809715695E-4</v>
+        <v>7.5398397546507803E-2</v>
       </c>
       <c r="F18">
-        <v>0.61315507631123001</v>
+        <v>3.7964934956685099E-3</v>
       </c>
       <c r="G18">
-        <v>0.99734399315384603</v>
+        <v>3.8471134089440903E-2</v>
       </c>
       <c r="H18">
-        <v>-1.99183507290868</v>
+        <v>7.3093565963403604</v>
       </c>
       <c r="I18">
-        <v>-8.5116287930899794</v>
+        <v>8.1937535691923404</v>
       </c>
       <c r="J18">
-        <v>-0.63295277266619798</v>
+        <v>8.4641318944150807</v>
       </c>
       <c r="K18" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M18" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N18" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="O18" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="P18" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="Q18" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="R18" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="S18" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="T18" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="U18" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="V18" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="W18" t="s">
-        <v>164</v>
-      </c>
-      <c r="X18" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="B19">
-        <v>0.63830387749305495</v>
+        <v>0.84158262276233298</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19">
-        <v>4.8476849803422897E-3</v>
+        <v>0.73664082972814804</v>
       </c>
       <c r="E19">
-        <v>3.5693556476693498E-2</v>
+        <v>0.93116326736450294</v>
       </c>
       <c r="F19">
-        <v>0.67130103556288401</v>
+        <v>3.3909585414294602E-3</v>
       </c>
       <c r="G19">
-        <v>0.99734399315384603</v>
+        <v>3.6816121306948398E-2</v>
       </c>
       <c r="H19">
-        <v>-1.1582210283757299</v>
+        <v>-0.575524571556006</v>
       </c>
       <c r="I19">
-        <v>-7.98886589803897</v>
+        <v>0.96357848552667003</v>
       </c>
       <c r="J19">
-        <v>-0.92871427344596602</v>
+        <v>-8.2584052144998097</v>
       </c>
       <c r="K19" t="s">
         <v>10</v>
       </c>
       <c r="L19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N19" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="O19" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="P19" t="s">
         <v>4</v>
@@ -2326,69 +2453,72 @@
         <v>5</v>
       </c>
       <c r="R19" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="S19" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="T19" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="U19" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="V19" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="W19" t="s">
-        <v>167</v>
+        <v>171</v>
+      </c>
+      <c r="X19" s="1">
+        <v>7.9999999999999996E-126</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="B20">
-        <v>0.499583840144535</v>
+        <v>7.2481639745308902E-3</v>
       </c>
       <c r="C20">
-        <v>0.80520105844980505</v>
+        <v>6.5233475770777996E-2</v>
       </c>
       <c r="D20">
-        <v>0.77724509606977199</v>
+        <v>4.13867409188252E-3</v>
       </c>
       <c r="E20">
-        <v>0.941906394828814</v>
-      </c>
-      <c r="F20" s="1">
-        <v>4.9791338043466801E-6</v>
+        <v>3.49488034425635E-2</v>
+      </c>
+      <c r="F20">
+        <v>7.6196451775790302E-4</v>
       </c>
       <c r="G20">
-        <v>1.5136566765213899E-4</v>
+        <v>1.15818606699201E-2</v>
       </c>
       <c r="H20">
-        <v>-1.19550244080604</v>
+        <v>1.9857567108410701</v>
       </c>
       <c r="I20">
-        <v>0.49459485341559101</v>
+        <v>2.1019114521654099</v>
       </c>
       <c r="J20">
-        <v>-8.9273371687900003</v>
+        <v>2.2052206251475699</v>
       </c>
       <c r="K20" t="s">
         <v>1</v>
       </c>
       <c r="L20" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M20" t="s">
         <v>2</v>
       </c>
       <c r="N20" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="O20" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="P20" t="s">
         <v>4</v>
@@ -2397,72 +2527,81 @@
         <v>5</v>
       </c>
       <c r="R20" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="S20" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="T20" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="U20" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="V20" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="W20" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="X20" s="1">
-        <v>7.9999999999999996E-126</v>
+        <v>2.0000000000000001E-127</v>
+      </c>
+      <c r="Y20" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="Z20" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="B21">
-        <v>0.84158262276233298</v>
-      </c>
-      <c r="C21" t="s">
-        <v>10</v>
+        <v>7.7721414886593093E-2</v>
+      </c>
+      <c r="C21">
+        <v>0.39403838801529101</v>
       </c>
       <c r="D21">
-        <v>0.73664082972814804</v>
+        <v>6.6966251935410303E-4</v>
       </c>
       <c r="E21">
-        <v>0.93116326736450294</v>
+        <v>7.2706216387016902E-3</v>
       </c>
       <c r="F21">
-        <v>3.3909585414294602E-3</v>
+        <v>0.802801862068799</v>
       </c>
       <c r="G21">
-        <v>3.6816121306948398E-2</v>
+        <v>0.99734399315384603</v>
       </c>
       <c r="H21">
-        <v>-0.575524571556006</v>
+        <v>-1.2939683480611199</v>
       </c>
       <c r="I21">
-        <v>0.96357848552667003</v>
+        <v>-2.4960304829707498</v>
       </c>
       <c r="J21">
-        <v>-8.2584052144998097</v>
+        <v>0.16291296848838199</v>
       </c>
       <c r="K21" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L21" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="O21" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="P21" t="s">
         <v>4</v>
@@ -2471,57 +2610,63 @@
         <v>5</v>
       </c>
       <c r="R21" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="S21" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="T21" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="U21" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="V21" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="W21" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="X21" s="1">
-        <v>7.9999999999999996E-126</v>
+        <v>2.0000000000000001E-127</v>
+      </c>
+      <c r="Y21" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B22">
-        <v>0.14384867448504099</v>
+        <v>0.15046919958421101</v>
       </c>
       <c r="C22">
-        <v>0.49500867396323101</v>
-      </c>
-      <c r="D22">
-        <v>1.3655637512706599E-4</v>
+        <v>0.50299703861007805</v>
+      </c>
+      <c r="D22" s="1">
+        <v>9.2015719344879594E-5</v>
       </c>
       <c r="E22">
-        <v>2.0756569019314101E-3</v>
+        <v>1.7482986675527101E-3</v>
       </c>
       <c r="F22">
-        <v>0.41488494772587298</v>
+        <v>4.2026271586780697E-2</v>
       </c>
       <c r="G22">
-        <v>0.99734399315384603</v>
+        <v>0.24569204927656399</v>
       </c>
       <c r="H22">
-        <v>2.2228154966237401</v>
+        <v>-0.71432114294556903</v>
       </c>
       <c r="I22">
-        <v>5.7667004006173297</v>
+        <v>-1.94391886793681</v>
       </c>
       <c r="J22">
-        <v>1.10716004687229</v>
+        <v>-0.89870437805570702</v>
       </c>
       <c r="K22" t="s">
         <v>1</v>
@@ -2533,66 +2678,66 @@
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="O22" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="P22" t="s">
         <v>4</v>
       </c>
       <c r="Q22" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="R22" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="S22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="T22" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="U22" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="V22" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="W22" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B23">
-        <v>7.2481639745308902E-3</v>
+        <v>1.59419095125224E-2</v>
       </c>
       <c r="C23">
-        <v>6.5233475770777996E-2</v>
+        <v>0.11657521331032</v>
       </c>
       <c r="D23">
-        <v>4.13867409188252E-3</v>
+        <v>4.7339319761837301E-4</v>
       </c>
       <c r="E23">
-        <v>3.49488034425635E-2</v>
+        <v>5.5350589259994401E-3</v>
       </c>
       <c r="F23">
-        <v>7.6196451775790302E-4</v>
+        <v>7.1683472380685903E-3</v>
       </c>
       <c r="G23">
-        <v>1.15818606699201E-2</v>
+        <v>6.8099298761651605E-2</v>
       </c>
       <c r="H23">
-        <v>1.9857567108410701</v>
+        <v>2.5525300669321198</v>
       </c>
       <c r="I23">
-        <v>2.1019114521654099</v>
+        <v>3.6992945352937099</v>
       </c>
       <c r="J23">
-        <v>2.2052206251475699</v>
+        <v>2.5459242730252698</v>
       </c>
       <c r="K23" t="s">
         <v>1</v>
@@ -2601,13 +2746,13 @@
         <v>2</v>
       </c>
       <c r="M23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="O23" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="P23" t="s">
         <v>4</v>
@@ -2622,66 +2767,66 @@
         <v>7</v>
       </c>
       <c r="T23" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="U23" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="V23" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="W23" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="X23" s="1">
         <v>2.0000000000000001E-127</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B24">
-        <v>0.882833179544669</v>
+        <v>2.7351902338559501E-2</v>
       </c>
       <c r="C24">
-        <v>0.96475623820401102</v>
+        <v>0.16843013545323501</v>
       </c>
       <c r="D24">
-        <v>0.217563022329992</v>
+        <v>3.1860298969465302E-4</v>
       </c>
       <c r="E24">
-        <v>0.663330614873758</v>
+        <v>4.0356378694656001E-3</v>
       </c>
       <c r="F24">
-        <v>2.0154616143659401E-3</v>
+        <v>2.3968772804732901E-2</v>
       </c>
       <c r="G24">
-        <v>2.55291804486352E-2</v>
+        <v>0.16371997829538501</v>
       </c>
       <c r="H24">
-        <v>0.23435948789918301</v>
+        <v>1.96513005696655</v>
       </c>
       <c r="I24">
-        <v>1.9524457757283</v>
+        <v>3.2030747455898201</v>
       </c>
       <c r="J24">
-        <v>-4.5117092967102197</v>
+        <v>1.79727972128311</v>
       </c>
       <c r="K24" t="s">
         <v>1</v>
       </c>
       <c r="L24" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="O24" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="P24" t="s">
         <v>4</v>
@@ -2696,66 +2841,75 @@
         <v>7</v>
       </c>
       <c r="T24" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="U24" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="V24" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="W24" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="X24" s="1">
         <v>2.0000000000000001E-127</v>
       </c>
+      <c r="Y24" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z24" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>197</v>
+      </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>108</v>
-      </c>
-      <c r="B25" s="1">
-        <v>7.2645747956430099E-25</v>
-      </c>
-      <c r="C25" s="1">
-        <v>8.4995525109023298E-23</v>
+        <v>63</v>
+      </c>
+      <c r="B25">
+        <v>0.59236535586476802</v>
+      </c>
+      <c r="C25">
+        <v>0.82508031709735496</v>
       </c>
       <c r="D25" s="1">
-        <v>2.0480265280941298E-24</v>
+        <v>7.3159683662301102E-12</v>
       </c>
       <c r="E25" s="1">
-        <v>3.1130003227030799E-22</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1.8435208765420901E-22</v>
-      </c>
-      <c r="G25" s="1">
-        <v>2.8021517323439703E-20</v>
+        <v>5.5601359583348798E-10</v>
+      </c>
+      <c r="F25">
+        <v>0.59169621019125596</v>
+      </c>
+      <c r="G25">
+        <v>0.99734399315384603</v>
       </c>
       <c r="H25">
-        <v>25.799031949536499</v>
+        <v>1.32814261145793</v>
       </c>
       <c r="I25">
-        <v>25.541920612953898</v>
+        <v>-19.635551971128599</v>
       </c>
       <c r="J25">
-        <v>22.460961767105299</v>
+        <v>1.1888044721057001</v>
       </c>
       <c r="K25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L25" t="s">
         <v>2</v>
       </c>
       <c r="M25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="O25" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="P25" t="s">
         <v>4</v>
@@ -2764,54 +2918,54 @@
         <v>5</v>
       </c>
       <c r="R25" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="S25" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="T25" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="U25" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="V25" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="W25" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="B26">
-        <v>0.59236535586476802</v>
+        <v>1.2817162989086099E-2</v>
       </c>
       <c r="C26">
-        <v>0.82508031709735496</v>
-      </c>
-      <c r="D26" s="1">
-        <v>7.3159683662301102E-12</v>
-      </c>
-      <c r="E26" s="1">
-        <v>5.5601359583348798E-10</v>
+        <v>9.9973871314871704E-2</v>
+      </c>
+      <c r="D26">
+        <v>1.65429974700948E-4</v>
+      </c>
+      <c r="E26">
+        <v>2.2859414685949199E-3</v>
       </c>
       <c r="F26">
-        <v>0.59169621019125596</v>
+        <v>3.7030354202105001E-2</v>
       </c>
       <c r="G26">
-        <v>0.99734399315384603</v>
+        <v>0.23452557661333201</v>
       </c>
       <c r="H26">
-        <v>1.32814261145793</v>
+        <v>2.18507826299735</v>
       </c>
       <c r="I26">
-        <v>-19.635551971128599</v>
+        <v>3.2942001927592499</v>
       </c>
       <c r="J26">
-        <v>1.1888044721057001</v>
+        <v>1.6339460315015999</v>
       </c>
       <c r="K26" t="s">
         <v>1</v>
@@ -2823,217 +2977,215 @@
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="O26" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="P26" t="s">
         <v>4</v>
       </c>
       <c r="Q26" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="R26" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="S26" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="T26" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="U26" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="V26" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="W26" t="s">
-        <v>167</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="Y26" s="2"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="B27">
-        <v>8.5320776887851096E-3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27">
-        <v>3.48720690711513E-3</v>
+        <v>0.16668498818429101</v>
+      </c>
+      <c r="C27">
+        <v>0.520079900515794</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2.2145186766993099E-5</v>
       </c>
       <c r="E27">
-        <v>3.11797323459705E-2</v>
+        <v>5.6101139809715695E-4</v>
       </c>
       <c r="F27">
-        <v>1.71192850067222E-3</v>
+        <v>0.61315507631123001</v>
       </c>
       <c r="G27">
-        <v>2.36557392820161E-2</v>
+        <v>0.99734399315384603</v>
       </c>
       <c r="H27">
-        <v>8.2400067398754295</v>
+        <v>-1.99183507290868</v>
       </c>
       <c r="I27">
-        <v>9.1230836510590603</v>
+        <v>-8.5116287930899794</v>
       </c>
       <c r="J27">
-        <v>8.9116972443720694</v>
+        <v>-0.63295277266619798</v>
       </c>
       <c r="K27" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L27" t="s">
         <v>2</v>
       </c>
       <c r="M27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N27" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="O27" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="P27" t="s">
         <v>4</v>
       </c>
       <c r="Q27" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="R27" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="S27" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="T27" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="U27" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="V27" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="W27" t="s">
-        <v>181</v>
-      </c>
-      <c r="X27" s="1">
-        <v>2.0000000000000001E-127</v>
+        <v>164</v>
+      </c>
+      <c r="X27" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="B28">
-        <v>5.2296258790457699E-4</v>
+        <v>0.14384867448504099</v>
       </c>
       <c r="C28">
-        <v>6.7985136427595001E-3</v>
+        <v>0.49500867396323101</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>1.3655637512706599E-4</v>
       </c>
       <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28" s="1">
-        <v>3.5239219193501199E-5</v>
+        <v>2.0756569019314101E-3</v>
+      </c>
+      <c r="F28">
+        <v>0.41488494772587298</v>
       </c>
       <c r="G28">
-        <v>7.6519447391602705E-4</v>
+        <v>0.99734399315384603</v>
       </c>
       <c r="H28">
-        <v>9.5195379091599097</v>
+        <v>2.2228154966237401</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>5.7667004006173297</v>
       </c>
       <c r="J28">
-        <v>10.366478918685701</v>
+        <v>1.10716004687229</v>
       </c>
       <c r="K28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L28" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N28" t="s">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="O28" t="s">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="P28" t="s">
         <v>4</v>
       </c>
       <c r="Q28" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="R28" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="S28" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="T28" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="U28" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="V28" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="W28" t="s">
-        <v>150</v>
-      </c>
-      <c r="X28" s="1">
-        <v>7.9999999999999996E-126</v>
+        <v>167</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="B29">
-        <v>0.73087028011701705</v>
-      </c>
-      <c r="C29" t="s">
-        <v>10</v>
+        <v>0.32671958514110599</v>
+      </c>
+      <c r="C29">
+        <v>0.69627656975421404</v>
       </c>
       <c r="D29">
-        <v>1.54082605663626E-3</v>
+        <v>4.9313466184905501E-3</v>
       </c>
       <c r="E29">
-        <v>1.5381297540471101E-2</v>
+        <v>3.5693556476693498E-2</v>
       </c>
       <c r="F29">
-        <v>0.72874036337219805</v>
+        <v>0.19886179858355699</v>
       </c>
       <c r="G29">
-        <v>0.99734399315384603</v>
+        <v>0.82528948433412697</v>
       </c>
       <c r="H29">
-        <v>-0.58724321488165099</v>
+        <v>0.77767918783579904</v>
       </c>
       <c r="I29">
-        <v>-6.9757384231914203</v>
+        <v>2.2213888527322601</v>
       </c>
       <c r="J29">
-        <v>0.51828966748271599</v>
+        <v>0.908460508709656</v>
       </c>
       <c r="K29" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L29" t="s">
         <v>2</v>
@@ -3042,10 +3194,10 @@
         <v>1</v>
       </c>
       <c r="N29" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="O29" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="P29" t="s">
         <v>4</v>
@@ -3054,72 +3206,69 @@
         <v>5</v>
       </c>
       <c r="R29" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="S29" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="T29" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="U29" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="V29" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="W29" t="s">
-        <v>184</v>
-      </c>
-      <c r="X29" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="B30">
-        <v>0.68913736661825598</v>
-      </c>
-      <c r="C30" t="s">
-        <v>10</v>
+        <v>0.18115724139428399</v>
+      </c>
+      <c r="C30">
+        <v>0.52988493107828105</v>
       </c>
       <c r="D30">
-        <v>1.61908395162854E-3</v>
+        <v>5.0265572576471899E-2</v>
       </c>
       <c r="E30">
-        <v>1.5381297540471101E-2</v>
+        <v>0.231526273685568</v>
       </c>
       <c r="F30">
-        <v>0.87396767139879195</v>
+        <v>2.5200208004161201E-3</v>
       </c>
       <c r="G30">
-        <v>0.99734399315384603</v>
+        <v>2.9464858589480801E-2</v>
       </c>
       <c r="H30">
-        <v>-0.68745418612221099</v>
+        <v>0.92791339438389997</v>
       </c>
       <c r="I30">
-        <v>-6.9635184693634002</v>
+        <v>-1.3818296697146699</v>
       </c>
       <c r="J30">
-        <v>0.23838138054142299</v>
+        <v>1.8550138623057999</v>
       </c>
       <c r="K30" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M30" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N30" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="O30" t="s">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="P30" t="s">
         <v>4</v>
@@ -3140,57 +3289,57 @@
         <v>9</v>
       </c>
       <c r="V30" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="W30" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="1">
-        <v>4.0166138013074299E-8</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1.5664793825099E-6</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1.5798540859477E-9</v>
-      </c>
-      <c r="E31" s="1">
-        <v>6.00344552660125E-8</v>
-      </c>
-      <c r="F31" s="1">
-        <v>7.1257924430440104E-7</v>
-      </c>
-      <c r="G31" s="1">
-        <v>2.7078011283567201E-5</v>
+        <v>17</v>
+      </c>
+      <c r="B31">
+        <v>0.882833179544669</v>
+      </c>
+      <c r="C31">
+        <v>0.96475623820401102</v>
+      </c>
+      <c r="D31">
+        <v>0.217563022329992</v>
+      </c>
+      <c r="E31">
+        <v>0.663330614873758</v>
+      </c>
+      <c r="F31">
+        <v>2.0154616143659401E-3</v>
+      </c>
+      <c r="G31">
+        <v>2.55291804486352E-2</v>
       </c>
       <c r="H31">
-        <v>9.8472328222506906</v>
+        <v>0.23435948789918301</v>
       </c>
       <c r="I31">
-        <v>10.7926616939578</v>
+        <v>1.9524457757283</v>
       </c>
       <c r="J31">
-        <v>8.3623201898607995</v>
+        <v>-4.5117092967102197</v>
       </c>
       <c r="K31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M31" t="s">
         <v>2</v>
       </c>
       <c r="N31" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="O31" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="P31" t="s">
         <v>4</v>
@@ -3205,66 +3354,66 @@
         <v>7</v>
       </c>
       <c r="T31" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="U31" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="V31" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="W31" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="X31" s="1">
-        <v>7.9999999999999996E-126</v>
+        <v>2.0000000000000001E-127</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32" s="1">
-        <v>4.3944727825824598E-5</v>
+        <v>11</v>
+      </c>
+      <c r="B32">
+        <v>0.499583840144535</v>
       </c>
       <c r="C32">
-        <v>8.5692219260358096E-4</v>
-      </c>
-      <c r="D32" s="1">
-        <v>2.0440309336398101E-5</v>
+        <v>0.80520105844980505</v>
+      </c>
+      <c r="D32">
+        <v>0.77724509606977199</v>
       </c>
       <c r="E32">
-        <v>5.6101139809715695E-4</v>
-      </c>
-      <c r="F32">
-        <v>2.7061485275990899E-4</v>
+        <v>0.941906394828814</v>
+      </c>
+      <c r="F32" s="1">
+        <v>4.9791338043466801E-6</v>
       </c>
       <c r="G32">
-        <v>5.1416822024382804E-3</v>
+        <v>1.5136566765213899E-4</v>
       </c>
       <c r="H32">
-        <v>10.0440404270764</v>
+        <v>-1.19550244080604</v>
       </c>
       <c r="I32">
-        <v>10.459349191909601</v>
+        <v>0.49459485341559101</v>
       </c>
       <c r="J32">
-        <v>8.2325208374458594</v>
+        <v>-8.9273371687900003</v>
       </c>
       <c r="K32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M32" t="s">
         <v>2</v>
       </c>
       <c r="N32" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="O32" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="P32" t="s">
         <v>4</v>
@@ -3273,32 +3422,51 @@
         <v>5</v>
       </c>
       <c r="R32" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="S32" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="T32" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="U32" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="V32" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="W32" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="X32" s="1">
-        <v>2.0000000000000001E-127</v>
+        <v>7.9999999999999996E-126</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W32">
-    <sortCondition ref="A2:A32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA32">
+    <sortCondition descending="1" ref="K2:K32"/>
+    <sortCondition descending="1" ref="L2:L32"/>
+    <sortCondition descending="1" ref="M2:M32"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="Y6" r:id="rId1" xr:uid="{C584BFB7-9B08-471E-A491-6BB48AEEF7B1}"/>
+    <hyperlink ref="Y21" r:id="rId2" xr:uid="{3785F14D-A746-4AFD-B218-39A601E1EF60}"/>
+    <hyperlink ref="Y24" r:id="rId3" display="https://link.springer.com/article/10.1007/s00338-021-02062-5\" xr:uid="{25EAD7D2-DEA8-407D-9FA6-E20EF9EEF301}"/>
+    <hyperlink ref="Z24" r:id="rId4" xr:uid="{E9579925-6E2F-4E6E-BDC9-5DCB1DE593DC}"/>
+    <hyperlink ref="Y10" r:id="rId5" xr:uid="{9009495B-66E4-4145-BE25-7995B00D6DBD}"/>
+    <hyperlink ref="Y8" r:id="rId6" xr:uid="{5150C0FD-C269-42FB-8F1F-F8ED4841EFA9}"/>
+    <hyperlink ref="Z12" r:id="rId7" xr:uid="{3C369733-BD65-4B8B-829A-B741E6AA49A0}"/>
+    <hyperlink ref="Y12" r:id="rId8" xr:uid="{271F992E-34A9-4B1D-A18A-7E66D2D48102}"/>
+    <hyperlink ref="Z20" r:id="rId9" xr:uid="{F1FC5FE0-FDDE-4BDE-AE4E-D1AED80990CD}"/>
+    <hyperlink ref="Y20" r:id="rId10" display="https://www.frontiersin.org/articles/10.3389/fmicb.2016.00316/full" xr:uid="{E876DFF1-D4E7-4448-BF68-EBB0528D4753}"/>
+    <hyperlink ref="Y2" r:id="rId11" xr:uid="{BCE38A66-1E12-49FC-BA2C-CE06BBDFAB74}"/>
+    <hyperlink ref="Z14" r:id="rId12" xr:uid="{2FF89DB9-B044-4FD5-9216-E9CC670F86FD}"/>
+    <hyperlink ref="Y14" r:id="rId13" xr:uid="{86DC4512-B1A5-4652-B9D2-4759D424613C}"/>
+    <hyperlink ref="Y3" r:id="rId14" display="https://link.springer.com/article/10.1007/s00338-021-02062-5\" xr:uid="{5064231E-EF2E-49FC-8FDC-FB3F573AE7D1}"/>
+    <hyperlink ref="Z3" r:id="rId15" xr:uid="{CECF25CC-9BEB-47CB-9B0B-A3D6662E6FE3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>